<commit_message>
Add ETF list management tools and update ETF names
- Add automated ETF name synchronization from Excel
- Implement ETF list management tools for add/remove operations
- Update ETF names: KOTAKALPHA→ALPHA, KOTAKIT→IT, KOTAKNV20→NV20, KOTAKPSUBK→PSUBANK
- Remove unavailable ETF: KOTAKLOVOL
- Add comprehensive backup and restore functionality
- Preserve all historical trading data during name changes

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/etf-list.xlsx
+++ b/etf-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avikmodak/Documents/etf-shop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9FA33-797D-A74E-9D8D-561140F3A083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4A28FD-D8DD-2344-806B-4701B727A9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>CPSEETF</t>
   </si>
@@ -46,9 +46,6 @@
     <t>NIF100IETF</t>
   </si>
   <si>
-    <t>KOTAKLOVOL</t>
-  </si>
-  <si>
     <t>LOWVOLIETF</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>EQUAL50ADD</t>
   </si>
   <si>
-    <t>KOTAKALPHA</t>
-  </si>
-  <si>
     <t>AUTOBEES</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>ITBEES</t>
   </si>
   <si>
-    <t>KOTAKIT</t>
-  </si>
-  <si>
     <t>MOM100</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>HDFCPVTBAN</t>
   </si>
   <si>
-    <t>KOTAKPSUBK</t>
-  </si>
-  <si>
     <t>PSUBNKIETF</t>
   </si>
   <si>
@@ -169,9 +157,6 @@
     <t>ESG</t>
   </si>
   <si>
-    <t>KOTAKNV20</t>
-  </si>
-  <si>
     <t>NV20IETF</t>
   </si>
   <si>
@@ -197,6 +182,18 @@
   </si>
   <si>
     <t>GOLD1</t>
+  </si>
+  <si>
+    <t>ALPHA</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>PSUBANK</t>
+  </si>
+  <si>
+    <t>NV20</t>
   </si>
 </sst>
 </file>
@@ -459,10 +456,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A59"/>
+  <dimension ref="A1:A58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -479,7 +476,7 @@
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -554,212 +551,207 @@
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>